<commit_message>
add refer_index in daily_report
</commit_message>
<xml_diff>
--- a/design/valuex.xlsx
+++ b/design/valuex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Project\Project\ValueX\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{12DE5518-B5C3-4CFF-B948-2C8DC1A3EEC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{85C30BE0-D1F6-449E-B020-8504AEF6252F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>float4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>参照指数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>refer_index</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +196,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -345,7 +357,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,9 +683,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K10"/>
+  <dimension ref="B2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -875,31 +889,41 @@
         <v>0</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="12"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
+      <c r="B9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -910,11 +934,27 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:K2"/>
-    <mergeCell ref="C9:K9"/>
     <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C11:K11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>